<commit_message>
- Updated Helios & Islander Matrix - Updated Influence Data
</commit_message>
<xml_diff>
--- a/Documents/Islanders/Islanders Matrix.xlsx
+++ b/Documents/Islanders/Islanders Matrix.xlsx
@@ -2773,7 +2773,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AB27" sqref="AB27"/>
+      <selection pane="bottomLeft" activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4880,7 +4880,7 @@
       <c r="AF33" s="6"/>
       <c r="AG33" s="6"/>
       <c r="AH33" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI33" s="6"/>
       <c r="AJ33" s="6"/>

</xml_diff>